<commit_message>
Limpia repo, separa dlm y dlm interv
</commit_message>
<xml_diff>
--- a/datos/pronosticos_banxico.xlsx
+++ b/datos/pronosticos_banxico.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juanpablolopezescamilla/Desktop/Tesis/cache/variables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juanpablolopezescamilla/Desktop/Tesis/datos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA36181-3173-154A-81A3-722973CB9EEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5AC12DF-8415-2241-98D9-5EC68ECB8566}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{0826A72E-9C85-0D48-94C8-A2A8B261856B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" activeTab="1" xr2:uid="{0826A72E-9C85-0D48-94C8-A2A8B261856B}"/>
   </bookViews>
   <sheets>
     <sheet name="historicos" sheetId="1" r:id="rId1"/>
@@ -534,11 +534,11 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1851,8 +1851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{858092B7-DC16-BE4B-B2A1-18BDE89AB6B9}">
   <dimension ref="A1:G538"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C540" sqref="C540"/>
+    <sheetView tabSelected="1" topLeftCell="A511" workbookViewId="0">
+      <selection activeCell="D539" sqref="D539"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1861,12 +1861,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
       <c r="F1" t="s">
         <v>91</v>
       </c>
@@ -2021,12 +2021,12 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -2172,12 +2172,12 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
@@ -2322,12 +2322,12 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="7" t="s">
+      <c r="A37" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
@@ -2472,12 +2472,12 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="7" t="s">
+      <c r="A49" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="B49" s="7"/>
-      <c r="C49" s="7"/>
-      <c r="D49" s="7"/>
+      <c r="B49" s="6"/>
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
@@ -2622,12 +2622,12 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" s="7" t="s">
+      <c r="A61" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="B61" s="7"/>
-      <c r="C61" s="7"/>
-      <c r="D61" s="7"/>
+      <c r="B61" s="6"/>
+      <c r="C61" s="6"/>
+      <c r="D61" s="6"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
@@ -2719,8 +2719,8 @@
         <v>17230.445020985651</v>
       </c>
       <c r="D67" s="5">
-        <f>((1+3.39/100)^(1/4)-1)*100</f>
-        <v>0.83693436649967534</v>
+        <f>((1+3.73/100)^(1/4)-1)*100</f>
+        <v>0.91973337769959418</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
@@ -2735,8 +2735,8 @@
         <v>17174.980213990544</v>
       </c>
       <c r="D68" s="5">
-        <f t="shared" ref="D68:D69" si="2">((1+3.39/100)^(1/4)-1)*100</f>
-        <v>0.83693436649967534</v>
+        <f>((1+3.73/100)^(1/4)-1)*100</f>
+        <v>0.91973337769959418</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
@@ -2751,8 +2751,8 @@
         <v>17944.703462191279</v>
       </c>
       <c r="D69" s="5">
-        <f t="shared" si="2"/>
-        <v>0.83693436649967534</v>
+        <f>((1+3.73/100)^(1/4)-1)*100</f>
+        <v>0.91973337769959418</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
@@ -2767,17 +2767,17 @@
         <v>17005.782449038721</v>
       </c>
       <c r="D70" s="5">
-        <f>((1+3.3/100)^(1/4)-1)*100</f>
-        <v>0.81498280423168978</v>
+        <f>((1+3.53/100)^(1/4)-1)*100</f>
+        <v>0.87105277245269619</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="7" t="s">
+      <c r="A73" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="B73" s="7"/>
-      <c r="C73" s="7"/>
-      <c r="D73" s="7"/>
+      <c r="B73" s="6"/>
+      <c r="C73" s="6"/>
+      <c r="D73" s="6"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
@@ -2869,8 +2869,8 @@
         <v>17130.272300920296</v>
       </c>
       <c r="D79" s="5">
-        <f>((1+3.25/100)^(1/4)-1)*100</f>
-        <v>0.80278129323012593</v>
+        <f>((1+3.78/100)^(1/4)-1)*100</f>
+        <v>0.93189252843739467</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
@@ -2885,8 +2885,8 @@
         <v>17927.43664687033</v>
       </c>
       <c r="D80" s="5">
-        <f>((1+3.25/100)^(1/4)-1)*100</f>
-        <v>0.80278129323012593</v>
+        <f>((1+3.78/100)^(1/4)-1)*100</f>
+        <v>0.93189252843739467</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
@@ -2901,8 +2901,8 @@
         <v>17046.661437514489</v>
       </c>
       <c r="D81" s="5">
-        <f>((1+3.27/100)^(1/4)-1)*100</f>
-        <v>0.80766242930203624</v>
+        <f>((1+3.52/100)^(1/4)-1)*100</f>
+        <v>0.8686168913875969</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
@@ -2917,17 +2917,17 @@
         <v>17656.150824450946</v>
       </c>
       <c r="D82" s="5">
-        <f>((1+3.27/100)^(1/4)-1)*100</f>
-        <v>0.80766242930203624</v>
+        <f>((1+3.52/100)^(1/4)-1)*100</f>
+        <v>0.8686168913875969</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A85" s="7" t="s">
+      <c r="A85" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="B85" s="7"/>
-      <c r="C85" s="7"/>
-      <c r="D85" s="7"/>
+      <c r="B85" s="6"/>
+      <c r="C85" s="6"/>
+      <c r="D85" s="6"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
@@ -3072,12 +3072,12 @@
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A97" s="7" t="s">
+      <c r="A97" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B97" s="7"/>
-      <c r="C97" s="7"/>
-      <c r="D97" s="7"/>
+      <c r="B97" s="6"/>
+      <c r="C97" s="6"/>
+      <c r="D97" s="6"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
@@ -3169,8 +3169,8 @@
         <v>16806.612606248997</v>
       </c>
       <c r="D103" s="5">
-        <f>((1+3.19/100)^(1/4)-1)*100</f>
-        <v>0.78813362900005401</v>
+        <f>((1+3.53/100)^(1/4)-1)*100</f>
+        <v>0.87105277245269619</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
@@ -3185,8 +3185,8 @@
         <v>17560.8971355635</v>
       </c>
       <c r="D104" s="5">
-        <f>((1+3.19/100)^(1/4)-1)*100</f>
-        <v>0.78813362900005401</v>
+        <f>((1+3.53/100)^(1/4)-1)*100</f>
+        <v>0.87105277245269619</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
@@ -3201,8 +3201,8 @@
         <v>17426.151251514591</v>
       </c>
       <c r="D105" s="5">
-        <f>((1+3.19/100)^(1/4)-1)*100</f>
-        <v>0.78813362900005401</v>
+        <f>((1+3.53/100)^(1/4)-1)*100</f>
+        <v>0.87105277245269619</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
@@ -3217,17 +3217,17 @@
         <v>18176.655887206416</v>
       </c>
       <c r="D106" s="5">
-        <f>((1+3.19/100)^(1/4)-1)*100</f>
-        <v>0.78813362900005401</v>
+        <f>((1+3.53/100)^(1/4)-1)*100</f>
+        <v>0.87105277245269619</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A109" s="7" t="s">
+      <c r="A109" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="B109" s="7"/>
-      <c r="C109" s="7"/>
-      <c r="D109" s="7"/>
+      <c r="B109" s="6"/>
+      <c r="C109" s="6"/>
+      <c r="D109" s="6"/>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
@@ -3372,12 +3372,12 @@
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A121" s="7" t="s">
+      <c r="A121" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="B121" s="7"/>
-      <c r="C121" s="7"/>
-      <c r="D121" s="7"/>
+      <c r="B121" s="6"/>
+      <c r="C121" s="6"/>
+      <c r="D121" s="6"/>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
@@ -3469,8 +3469,8 @@
         <v>17315.28514536345</v>
       </c>
       <c r="D127" s="5">
-        <f>((1+3.2/100)^(1/4)-1)*100</f>
-        <v>0.79057534988196121</v>
+        <f>((1+3.5/100)^(1/4)-1)*100</f>
+        <v>0.86374459977134332</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
@@ -3485,8 +3485,8 @@
         <v>18117.262257377057</v>
       </c>
       <c r="D128" s="5">
-        <f>((1+3.2/100)^(1/4)-1)*100</f>
-        <v>0.79057534988196121</v>
+        <f>((1+3.5/100)^(1/4)-1)*100</f>
+        <v>0.86374459977134332</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
@@ -3501,8 +3501,8 @@
         <v>17474.154492618614</v>
       </c>
       <c r="D129" s="5">
-        <f>((1+3.19/100)^(1/4)-1)*100</f>
-        <v>0.78813362900005401</v>
+        <f>((1+3.55/100)^(1/4)-1)*100</f>
+        <v>0.87592400524596492</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
@@ -3517,17 +3517,17 @@
         <v>18109.700683409035</v>
       </c>
       <c r="D130" s="5">
-        <f>((1+3.19/100)^(1/4)-1)*100</f>
-        <v>0.78813362900005401</v>
+        <f>((1+3.55/100)^(1/4)-1)*100</f>
+        <v>0.87592400524596492</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A133" s="7" t="s">
+      <c r="A133" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="B133" s="7"/>
-      <c r="C133" s="7"/>
-      <c r="D133" s="7"/>
+      <c r="B133" s="6"/>
+      <c r="C133" s="6"/>
+      <c r="D133" s="6"/>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
@@ -3651,7 +3651,7 @@
         <v>18125.383270068334</v>
       </c>
       <c r="D141" s="5">
-        <f t="shared" ref="D141:D142" si="3">((1+3.49/100)^(1/4)-1)*100</f>
+        <f t="shared" ref="D141:D142" si="2">((1+3.49/100)^(1/4)-1)*100</f>
         <v>0.86130818916048124</v>
       </c>
     </row>
@@ -3667,17 +3667,17 @@
         <v>17982.498922309464</v>
       </c>
       <c r="D142" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.86130818916048124</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A145" s="7" t="s">
+      <c r="A145" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="B145" s="7"/>
-      <c r="C145" s="7"/>
-      <c r="D145" s="7"/>
+      <c r="B145" s="6"/>
+      <c r="C145" s="6"/>
+      <c r="D145" s="6"/>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
@@ -3769,8 +3769,8 @@
         <v>17333.261763631061</v>
       </c>
       <c r="D151" s="5">
-        <f>((1+3.24/100)^(1/4)-1)*100</f>
-        <v>0.80034045926844488</v>
+        <f>((1+3.52/100)^(1/4)-1)*100</f>
+        <v>0.8686168913875969</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
@@ -3785,8 +3785,8 @@
         <v>18014.007838155067</v>
       </c>
       <c r="D152" s="5">
-        <f t="shared" ref="D152:D154" si="4">((1+3.24/100)^(1/4)-1)*100</f>
-        <v>0.80034045926844488</v>
+        <f t="shared" ref="D152:D154" si="3">((1+3.52/100)^(1/4)-1)*100</f>
+        <v>0.8686168913875969</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
@@ -3801,8 +3801,8 @@
         <v>17906.450858743854</v>
       </c>
       <c r="D153" s="5">
-        <f t="shared" si="4"/>
-        <v>0.80034045926844488</v>
+        <f t="shared" si="3"/>
+        <v>0.8686168913875969</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
@@ -3817,17 +3817,17 @@
         <v>18751.378592015677</v>
       </c>
       <c r="D154" s="5">
-        <f t="shared" si="4"/>
-        <v>0.80034045926844488</v>
+        <f t="shared" si="3"/>
+        <v>0.8686168913875969</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A157" s="7" t="s">
+      <c r="A157" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="B157" s="7"/>
-      <c r="C157" s="7"/>
-      <c r="D157" s="7"/>
+      <c r="B157" s="6"/>
+      <c r="C157" s="6"/>
+      <c r="D157" s="6"/>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
@@ -3919,8 +3919,8 @@
         <v>17844.119735103726</v>
       </c>
       <c r="D163" s="5">
-        <f>((1+3.13/100)^(1/4)-1)*100</f>
-        <v>0.77347957569464665</v>
+        <f>((1+3.46/100)^(1/4)-1)*100</f>
+        <v>0.85399789775877366</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.2">
@@ -3935,8 +3935,8 @@
         <v>17754.819263690173</v>
       </c>
       <c r="D164" s="5">
-        <f>((1+3.13/100)^(1/4)-1)*100</f>
-        <v>0.77347957569464665</v>
+        <f>((1+3.46/100)^(1/4)-1)*100</f>
+        <v>0.85399789775877366</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.2">
@@ -3951,8 +3951,8 @@
         <v>18603.57772042849</v>
       </c>
       <c r="D165" s="5">
-        <f>((1+3.13/100)^(1/4)-1)*100</f>
-        <v>0.77347957569464665</v>
+        <f>((1+3.46/100)^(1/4)-1)*100</f>
+        <v>0.85399789775877366</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.2">
@@ -3967,17 +3967,17 @@
         <v>17919.295122023672</v>
       </c>
       <c r="D166" s="5">
-        <f>((1+3.19/100)^(1/4)-1)*100</f>
-        <v>0.78813362900005401</v>
+        <f>((1+3.49/100)^(1/4)-1)*100</f>
+        <v>0.86130818916048124</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A169" s="7" t="s">
+      <c r="A169" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="B169" s="7"/>
-      <c r="C169" s="7"/>
-      <c r="D169" s="7"/>
+      <c r="B169" s="6"/>
+      <c r="C169" s="6"/>
+      <c r="D169" s="6"/>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
@@ -4069,8 +4069,8 @@
         <v>17648.334525608105</v>
       </c>
       <c r="D175" s="5">
-        <f>((1+3.06/100)^(1/4)-1)*100</f>
-        <v>0.75637509640957834</v>
+        <f>((1+3.36/100)^(1/4)-1)*100</f>
+        <v>0.8296187720209014</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.2">
@@ -4085,8 +4085,8 @@
         <v>18479.531300219449</v>
       </c>
       <c r="D176" s="5">
-        <f>((1+3.06/100)^(1/4)-1)*100</f>
-        <v>0.75637509640957834</v>
+        <f>((1+3.36/100)^(1/4)-1)*100</f>
+        <v>0.8296187720209014</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.2">
@@ -4101,8 +4101,8 @@
         <v>17815.463293111457</v>
       </c>
       <c r="D177" s="5">
-        <f>((1+3.15/100)^(1/4)-1)*100</f>
-        <v>0.77836497042846897</v>
+        <f>((1+3.4/100)^(1/4)-1)*100</f>
+        <v>0.83937254420483054</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.2">
@@ -4117,17 +4117,17 @@
         <v>18481.643092769023</v>
       </c>
       <c r="D178" s="5">
-        <f>((1+3.15/100)^(1/4)-1)*100</f>
-        <v>0.77836497042846897</v>
+        <f>((1+3.4/100)^(1/4)-1)*100</f>
+        <v>0.83937254420483054</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A181" s="7" t="s">
+      <c r="A181" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="B181" s="7"/>
-      <c r="C181" s="7"/>
-      <c r="D181" s="7"/>
+      <c r="B181" s="6"/>
+      <c r="C181" s="6"/>
+      <c r="D181" s="6"/>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
@@ -4272,12 +4272,12 @@
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A193" s="7" t="s">
+      <c r="A193" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="B193" s="7"/>
-      <c r="C193" s="7"/>
-      <c r="D193" s="7"/>
+      <c r="B193" s="6"/>
+      <c r="C193" s="6"/>
+      <c r="D193" s="6"/>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
@@ -4422,12 +4422,12 @@
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A205" s="7" t="s">
+      <c r="A205" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="B205" s="7"/>
-      <c r="C205" s="7"/>
-      <c r="D205" s="7"/>
+      <c r="B205" s="6"/>
+      <c r="C205" s="6"/>
+      <c r="D205" s="6"/>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
@@ -4519,8 +4519,8 @@
         <v>18191.705432918141</v>
       </c>
       <c r="D211" s="5">
-        <f>((1+3.2/100)^(1/4)-1)*100</f>
-        <v>0.79057534988196121</v>
+        <f>((1+3.41/100)^(1/4)-1)*100</f>
+        <v>0.84181054506595743</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.2">
@@ -4535,8 +4535,8 @@
         <v>18271.115531283533</v>
       </c>
       <c r="D212" s="5">
-        <f>((1+3.2/100)^(1/4)-1)*100</f>
-        <v>0.79057534988196121</v>
+        <f t="shared" ref="D212:D213" si="4">((1+3.41/100)^(1/4)-1)*100</f>
+        <v>0.84181054506595743</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.2">
@@ -4551,8 +4551,8 @@
         <v>18877.00818728864</v>
       </c>
       <c r="D213" s="5">
-        <f>((1+3.2/100)^(1/4)-1)*100</f>
-        <v>0.79057534988196121</v>
+        <f t="shared" si="4"/>
+        <v>0.84181054506595743</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.2">
@@ -4567,17 +4567,17 @@
         <v>18234.746735354511</v>
       </c>
       <c r="D214" s="5">
-        <f>((1+3.25/100)^(1/4)-1)*100</f>
-        <v>0.80278129323012593</v>
+        <f>((1+3.5/100)^(1/4)-1)*100</f>
+        <v>0.86374459977134332</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A217" s="7" t="s">
+      <c r="A217" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="B217" s="7"/>
-      <c r="C217" s="7"/>
-      <c r="D217" s="7"/>
+      <c r="B217" s="6"/>
+      <c r="C217" s="6"/>
+      <c r="D217" s="6"/>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
@@ -4669,8 +4669,8 @@
         <v>18210.650245901372</v>
       </c>
       <c r="D223" s="5">
-        <f>((1+3.22/100)^(1/4)-1)*100</f>
-        <v>0.79545825934328462</v>
+        <f>((1+3.39/100)^(1/4)-1)*100</f>
+        <v>0.83693436649967534</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.2">
@@ -4685,8 +4685,8 @@
         <v>18809.073436859777</v>
       </c>
       <c r="D224" s="5">
-        <f>((1+3.22/100)^(1/4)-1)*100</f>
-        <v>0.79545825934328462</v>
+        <f>((1+3.39/100)^(1/4)-1)*100</f>
+        <v>0.83693436649967534</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.2">
@@ -4701,8 +4701,8 @@
         <v>18133.829328336225</v>
       </c>
       <c r="D225" s="5">
-        <f>((1+3.26/100)^(1/4)-1)*100</f>
-        <v>0.8052219498979829</v>
+        <f>((1+3.42/100)^(1/4)-1)*100</f>
+        <v>0.84424836911300982</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.2">
@@ -4717,17 +4717,17 @@
         <v>18808.893910540875</v>
       </c>
       <c r="D226" s="5">
-        <f>((1+3.26/100)^(1/4)-1)*100</f>
-        <v>0.8052219498979829</v>
+        <f>((1+3.42/100)^(1/4)-1)*100</f>
+        <v>0.84424836911300982</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A229" s="7" t="s">
+      <c r="A229" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="B229" s="7"/>
-      <c r="C229" s="7"/>
-      <c r="D229" s="7"/>
+      <c r="B229" s="6"/>
+      <c r="C229" s="6"/>
+      <c r="D229" s="6"/>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
@@ -4872,12 +4872,12 @@
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A241" s="7" t="s">
+      <c r="A241" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="B241" s="7"/>
-      <c r="C241" s="7"/>
-      <c r="D241" s="7"/>
+      <c r="B241" s="6"/>
+      <c r="C241" s="6"/>
+      <c r="D241" s="6"/>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
@@ -5022,12 +5022,12 @@
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A253" s="7" t="s">
+      <c r="A253" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="B253" s="7"/>
-      <c r="C253" s="7"/>
-      <c r="D253" s="7"/>
+      <c r="B253" s="6"/>
+      <c r="C253" s="6"/>
+      <c r="D253" s="6"/>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
@@ -5172,12 +5172,12 @@
       </c>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A265" s="7" t="s">
+      <c r="A265" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="B265" s="7"/>
-      <c r="C265" s="7"/>
-      <c r="D265" s="7"/>
+      <c r="B265" s="6"/>
+      <c r="C265" s="6"/>
+      <c r="D265" s="6"/>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
@@ -5322,12 +5322,12 @@
       </c>
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A277" s="7" t="s">
+      <c r="A277" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="B277" s="7"/>
-      <c r="C277" s="7"/>
-      <c r="D277" s="7"/>
+      <c r="B277" s="6"/>
+      <c r="C277" s="6"/>
+      <c r="D277" s="6"/>
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
@@ -5472,12 +5472,12 @@
       </c>
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A289" s="7" t="s">
+      <c r="A289" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="B289" s="7"/>
-      <c r="C289" s="7"/>
-      <c r="D289" s="7"/>
+      <c r="B289" s="6"/>
+      <c r="C289" s="6"/>
+      <c r="D289" s="6"/>
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
@@ -5622,12 +5622,12 @@
       </c>
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A301" s="7" t="s">
+      <c r="A301" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="B301" s="7"/>
-      <c r="C301" s="7"/>
-      <c r="D301" s="7"/>
+      <c r="B301" s="6"/>
+      <c r="C301" s="6"/>
+      <c r="D301" s="6"/>
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
@@ -5772,12 +5772,12 @@
       </c>
     </row>
     <row r="313" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A313" s="7" t="s">
+      <c r="A313" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="B313" s="7"/>
-      <c r="C313" s="7"/>
-      <c r="D313" s="7"/>
+      <c r="B313" s="6"/>
+      <c r="C313" s="6"/>
+      <c r="D313" s="6"/>
     </row>
     <row r="314" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
@@ -5922,12 +5922,12 @@
       </c>
     </row>
     <row r="325" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A325" s="7" t="s">
+      <c r="A325" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="B325" s="7"/>
-      <c r="C325" s="7"/>
-      <c r="D325" s="7"/>
+      <c r="B325" s="6"/>
+      <c r="C325" s="6"/>
+      <c r="D325" s="6"/>
     </row>
     <row r="326" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
@@ -6072,12 +6072,12 @@
       </c>
     </row>
     <row r="337" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A337" s="7" t="s">
+      <c r="A337" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="B337" s="7"/>
-      <c r="C337" s="7"/>
-      <c r="D337" s="7"/>
+      <c r="B337" s="6"/>
+      <c r="C337" s="6"/>
+      <c r="D337" s="6"/>
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A338" t="s">
@@ -6222,12 +6222,12 @@
       </c>
     </row>
     <row r="349" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A349" s="7" t="s">
+      <c r="A349" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="B349" s="7"/>
-      <c r="C349" s="7"/>
-      <c r="D349" s="7"/>
+      <c r="B349" s="6"/>
+      <c r="C349" s="6"/>
+      <c r="D349" s="6"/>
     </row>
     <row r="350" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A350" t="s">
@@ -6372,12 +6372,12 @@
       </c>
     </row>
     <row r="361" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A361" s="7" t="s">
+      <c r="A361" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="B361" s="7"/>
-      <c r="C361" s="7"/>
-      <c r="D361" s="7"/>
+      <c r="B361" s="6"/>
+      <c r="C361" s="6"/>
+      <c r="D361" s="6"/>
     </row>
     <row r="362" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A362" t="s">
@@ -6522,12 +6522,12 @@
       </c>
     </row>
     <row r="373" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A373" s="7" t="s">
+      <c r="A373" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="B373" s="7"/>
-      <c r="C373" s="7"/>
-      <c r="D373" s="7"/>
+      <c r="B373" s="6"/>
+      <c r="C373" s="6"/>
+      <c r="D373" s="6"/>
     </row>
     <row r="374" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A374" t="s">
@@ -6672,12 +6672,12 @@
       </c>
     </row>
     <row r="385" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A385" s="7" t="s">
+      <c r="A385" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="B385" s="7"/>
-      <c r="C385" s="7"/>
-      <c r="D385" s="7"/>
+      <c r="B385" s="6"/>
+      <c r="C385" s="6"/>
+      <c r="D385" s="6"/>
     </row>
     <row r="386" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A386" t="s">
@@ -6822,12 +6822,12 @@
       </c>
     </row>
     <row r="397" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A397" s="7" t="s">
+      <c r="A397" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="B397" s="7"/>
-      <c r="C397" s="7"/>
-      <c r="D397" s="7"/>
+      <c r="B397" s="6"/>
+      <c r="C397" s="6"/>
+      <c r="D397" s="6"/>
     </row>
     <row r="398" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A398" t="s">
@@ -6967,17 +6967,17 @@
         <v>18320.248845324091</v>
       </c>
       <c r="D406" s="5">
-        <f>((1+0/100)^(1/4)-1)*100</f>
-        <v>0</v>
+        <f>((1+3.56/100)^(1/4)-1)*100</f>
+        <v>0.87835935703375334</v>
       </c>
     </row>
     <row r="409" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A409" s="7" t="s">
+      <c r="A409" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="B409" s="7"/>
-      <c r="C409" s="7"/>
-      <c r="D409" s="7"/>
+      <c r="B409" s="6"/>
+      <c r="C409" s="6"/>
+      <c r="D409" s="6"/>
     </row>
     <row r="410" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A410" t="s">
@@ -7122,12 +7122,12 @@
       </c>
     </row>
     <row r="421" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A421" s="7" t="s">
+      <c r="A421" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="B421" s="7"/>
-      <c r="C421" s="7"/>
-      <c r="D421" s="7"/>
+      <c r="B421" s="6"/>
+      <c r="C421" s="6"/>
+      <c r="D421" s="6"/>
     </row>
     <row r="422" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A422" t="s">
@@ -7277,12 +7277,12 @@
       <c r="D432" s="3"/>
     </row>
     <row r="433" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A433" s="7" t="s">
+      <c r="A433" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="B433" s="7"/>
-      <c r="C433" s="7"/>
-      <c r="D433" s="7"/>
+      <c r="B433" s="6"/>
+      <c r="C433" s="6"/>
+      <c r="D433" s="6"/>
     </row>
     <row r="434" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A434" t="s">
@@ -7437,12 +7437,12 @@
       <c r="D444" s="3"/>
     </row>
     <row r="445" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A445" s="7" t="s">
+      <c r="A445" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="B445" s="7"/>
-      <c r="C445" s="7"/>
-      <c r="D445" s="7"/>
+      <c r="B445" s="6"/>
+      <c r="C445" s="6"/>
+      <c r="D445" s="6"/>
     </row>
     <row r="446" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A446" t="s">
@@ -7597,12 +7597,12 @@
       <c r="D456" s="3"/>
     </row>
     <row r="457" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A457" s="7" t="s">
+      <c r="A457" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="B457" s="7"/>
-      <c r="C457" s="7"/>
-      <c r="D457" s="7"/>
+      <c r="B457" s="6"/>
+      <c r="C457" s="6"/>
+      <c r="D457" s="6"/>
     </row>
     <row r="458" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A458" t="s">
@@ -7757,12 +7757,12 @@
       <c r="D468" s="3"/>
     </row>
     <row r="469" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A469" s="7" t="s">
+      <c r="A469" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="B469" s="7"/>
-      <c r="C469" s="7"/>
-      <c r="D469" s="7"/>
+      <c r="B469" s="6"/>
+      <c r="C469" s="6"/>
+      <c r="D469" s="6"/>
     </row>
     <row r="470" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A470" t="s">
@@ -7917,12 +7917,12 @@
       <c r="D480" s="5"/>
     </row>
     <row r="481" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A481" s="7" t="s">
+      <c r="A481" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="B481" s="7"/>
-      <c r="C481" s="7"/>
-      <c r="D481" s="7"/>
+      <c r="B481" s="6"/>
+      <c r="C481" s="6"/>
+      <c r="D481" s="6"/>
     </row>
     <row r="482" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A482" t="s">
@@ -8014,8 +8014,8 @@
         <v>18430.642663977542</v>
       </c>
       <c r="D487" s="5">
-        <f>((1+3.64/100)^(1/4)-1)*100</f>
-        <v>0.89783582465745582</v>
+        <f>((1+3.72/100)^(1/4)-1)*100</f>
+        <v>0.91730102008877878</v>
       </c>
     </row>
     <row r="488" spans="1:4" x14ac:dyDescent="0.2">
@@ -8030,8 +8030,8 @@
         <v>18785.208310311737</v>
       </c>
       <c r="D488" s="5">
-        <f>((1+3.64/100)^(1/4)-1)*100</f>
-        <v>0.89783582465745582</v>
+        <f t="shared" ref="D488:D490" si="5">((1+3.72/100)^(1/4)-1)*100</f>
+        <v>0.91730102008877878</v>
       </c>
     </row>
     <row r="489" spans="1:4" x14ac:dyDescent="0.2">
@@ -8046,8 +8046,8 @@
         <v>18479.418335486709</v>
       </c>
       <c r="D489" s="5">
-        <f>((1+3.64/100)^(1/4)-1)*100</f>
-        <v>0.89783582465745582</v>
+        <f t="shared" si="5"/>
+        <v>0.91730102008877878</v>
       </c>
     </row>
     <row r="490" spans="1:4" x14ac:dyDescent="0.2">
@@ -8062,8 +8062,8 @@
         <v>19130.831191679365</v>
       </c>
       <c r="D490" s="5">
-        <f>((1+3.64/100)^(1/4)-1)*100</f>
-        <v>0.89783582465745582</v>
+        <f t="shared" si="5"/>
+        <v>0.91730102008877878</v>
       </c>
     </row>
     <row r="491" spans="1:4" x14ac:dyDescent="0.2">
@@ -8077,12 +8077,12 @@
       <c r="D492" s="5"/>
     </row>
     <row r="493" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A493" s="7" t="s">
+      <c r="A493" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B493" s="7"/>
-      <c r="C493" s="7"/>
-      <c r="D493" s="7"/>
+      <c r="B493" s="6"/>
+      <c r="C493" s="6"/>
+      <c r="D493" s="6"/>
     </row>
     <row r="494" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A494" t="s">
@@ -8227,12 +8227,12 @@
       </c>
     </row>
     <row r="505" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A505" s="7" t="s">
+      <c r="A505" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="B505" s="7"/>
-      <c r="C505" s="7"/>
-      <c r="D505" s="7"/>
+      <c r="B505" s="6"/>
+      <c r="C505" s="6"/>
+      <c r="D505" s="6"/>
     </row>
     <row r="506" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A506" t="s">
@@ -8377,12 +8377,12 @@
       </c>
     </row>
     <row r="517" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A517" s="7" t="s">
+      <c r="A517" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="B517" s="7"/>
-      <c r="C517" s="7"/>
-      <c r="D517" s="7"/>
+      <c r="B517" s="6"/>
+      <c r="C517" s="6"/>
+      <c r="D517" s="6"/>
     </row>
     <row r="518" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A518" t="s">
@@ -8527,12 +8527,12 @@
       </c>
     </row>
     <row r="529" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A529" s="7" t="s">
+      <c r="A529" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="B529" s="7"/>
-      <c r="C529" s="7"/>
-      <c r="D529" s="7"/>
+      <c r="B529" s="6"/>
+      <c r="C529" s="6"/>
+      <c r="D529" s="6"/>
     </row>
     <row r="530" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A530" t="s">
@@ -8678,31 +8678,16 @@
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="A481:D481"/>
-    <mergeCell ref="A493:D493"/>
-    <mergeCell ref="A505:D505"/>
-    <mergeCell ref="A517:D517"/>
-    <mergeCell ref="A529:D529"/>
-    <mergeCell ref="A421:D421"/>
-    <mergeCell ref="A433:D433"/>
-    <mergeCell ref="A445:D445"/>
-    <mergeCell ref="A457:D457"/>
-    <mergeCell ref="A469:D469"/>
-    <mergeCell ref="A361:D361"/>
-    <mergeCell ref="A373:D373"/>
-    <mergeCell ref="A385:D385"/>
-    <mergeCell ref="A397:D397"/>
-    <mergeCell ref="A409:D409"/>
-    <mergeCell ref="A301:D301"/>
-    <mergeCell ref="A313:D313"/>
-    <mergeCell ref="A325:D325"/>
-    <mergeCell ref="A337:D337"/>
-    <mergeCell ref="A349:D349"/>
-    <mergeCell ref="A241:D241"/>
-    <mergeCell ref="A253:D253"/>
-    <mergeCell ref="A265:D265"/>
-    <mergeCell ref="A277:D277"/>
-    <mergeCell ref="A289:D289"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="A49:D49"/>
+    <mergeCell ref="A61:D61"/>
+    <mergeCell ref="A73:D73"/>
+    <mergeCell ref="A85:D85"/>
+    <mergeCell ref="A97:D97"/>
+    <mergeCell ref="A109:D109"/>
     <mergeCell ref="A121:D121"/>
     <mergeCell ref="A133:D133"/>
     <mergeCell ref="A145:D145"/>
@@ -8713,16 +8698,31 @@
     <mergeCell ref="A193:D193"/>
     <mergeCell ref="A205:D205"/>
     <mergeCell ref="A217:D217"/>
-    <mergeCell ref="A61:D61"/>
-    <mergeCell ref="A73:D73"/>
-    <mergeCell ref="A85:D85"/>
-    <mergeCell ref="A97:D97"/>
-    <mergeCell ref="A109:D109"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A37:D37"/>
-    <mergeCell ref="A49:D49"/>
+    <mergeCell ref="A241:D241"/>
+    <mergeCell ref="A253:D253"/>
+    <mergeCell ref="A265:D265"/>
+    <mergeCell ref="A277:D277"/>
+    <mergeCell ref="A289:D289"/>
+    <mergeCell ref="A301:D301"/>
+    <mergeCell ref="A313:D313"/>
+    <mergeCell ref="A325:D325"/>
+    <mergeCell ref="A337:D337"/>
+    <mergeCell ref="A349:D349"/>
+    <mergeCell ref="A361:D361"/>
+    <mergeCell ref="A373:D373"/>
+    <mergeCell ref="A385:D385"/>
+    <mergeCell ref="A397:D397"/>
+    <mergeCell ref="A409:D409"/>
+    <mergeCell ref="A421:D421"/>
+    <mergeCell ref="A433:D433"/>
+    <mergeCell ref="A445:D445"/>
+    <mergeCell ref="A457:D457"/>
+    <mergeCell ref="A469:D469"/>
+    <mergeCell ref="A481:D481"/>
+    <mergeCell ref="A493:D493"/>
+    <mergeCell ref="A505:D505"/>
+    <mergeCell ref="A517:D517"/>
+    <mergeCell ref="A529:D529"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>